<commit_message>
add case swapon 8,valgrind 5,overlayfs 4,oprofile 12,pktgen 9,powertop 11,slabtop 5
</commit_message>
<xml_diff>
--- a/list/tool.xlsx
+++ b/list/tool.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$166</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$196</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$I$101</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320">
   <si>
     <t>测试项目</t>
   </si>
@@ -1617,6 +1617,12 @@
     <t>memwatch</t>
   </si>
   <si>
+    <t>1. 下载安装包：http://www.linkdata.se/sourcecode/memwatch/</t>
+  </si>
+  <si>
+    <t>memwatch是C语言的内存检测器</t>
+  </si>
+  <si>
     <t>pidstat</t>
   </si>
   <si>
@@ -1666,6 +1672,9 @@
       </rPr>
       <t>pidstat</t>
     </r>
+  </si>
+  <si>
+    <t>pidstat.sh</t>
   </si>
   <si>
     <t>pidstat主要用于监控全部或指定进程占用系统资源的情况，如CPU，内存、设备IO、任务切换、线程等</t>
@@ -1864,6 +1873,9 @@
       </rPr>
       <t>: lspci</t>
     </r>
+  </si>
+  <si>
+    <t>setpci.md</t>
   </si>
   <si>
     <r>
@@ -2122,10 +2134,40 @@
     <t>swapon</t>
   </si>
   <si>
+    <t>1. 显示版本讯息：swapon -V</t>
+  </si>
+  <si>
+    <t>swapon.sh</t>
+  </si>
+  <si>
+    <t>2. enable all swaps：swapon -a</t>
+  </si>
+  <si>
+    <t>3.  enable swap discards: swapon -d</t>
+  </si>
+  <si>
+    <t>4. silently skip devices that do not exist: swapon -e</t>
+  </si>
+  <si>
+    <t>5.  display summary about used swap devices: swapon -s</t>
+  </si>
+  <si>
+    <t>6. 指定交换区的优先顺序: swapon -p -2</t>
+  </si>
+  <si>
+    <t>7. 关闭swap的指令:swapoff -a</t>
+  </si>
+  <si>
+    <t>8. display this help and exit: swapon --help</t>
+  </si>
+  <si>
     <t>sysdig</t>
   </si>
   <si>
     <t>1.install package: yum install -y kernel-devel* dkms sysdig</t>
+  </si>
+  <si>
+    <t>无sysdig安装包</t>
   </si>
   <si>
     <r>
@@ -2153,16 +2195,1148 @@
     <t>valgrind</t>
   </si>
   <si>
+    <t>1. install valgrind : yum install -y valgrind</t>
+  </si>
+  <si>
+    <t>valgrind.md</t>
+  </si>
+  <si>
+    <t>Valgrind是一套Linux下，开放源代码（GPL V2）的仿真调试工具的集合</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>查看内核版本：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>valgrind --version</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>检测内存泄露</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+a. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>创建</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">memleak.c
+#include &lt;stdlib.h&gt;
+#include &lt;stdio.h&gt;
+int main(void)
+{
+       char *ptr;
+       ptr = (char *)malloc(10);
+       return 0;
+}
+b. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>编译</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>memle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ak</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">.c
+$ gcc -o memleak memleak.c
+c. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>valgri</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>检测</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+$ va</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>lg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>rind --leak-check=full ./memleak</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>检测其它内存问题</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+a. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>创建</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">memcheck.c
+#include &lt;stdlib.h&gt;
+#include &lt;stdio.h&gt;
+int main(void)
+{
+    char *ptr = malloc(10);
+    ptr[12] = 'a'; // </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>内存越界</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">memcpy(ptr +1, ptr, 5); // </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>踩内存</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">  c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">har a[10];
+    a[12] = 'i'; // </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>数组越界</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">  fr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">ee(ptr); // </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>重复释放</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">   f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">ree(ptr);
+    char *p1;
+    *p1 = '1'; // </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非法指针</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+    ret</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">urn </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">0;
+}
+b. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>编译</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>memcheck.c
+$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> g</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>cc -o memcheck memcheck.c -g
+c. valgrind --leak-check=full ./memcheck</t>
+    </r>
+  </si>
+  <si>
+    <t>5. remove valgrind: yum remove -y valgrind</t>
+  </si>
+  <si>
     <t>overlayfs</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>加载</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>overlayfs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>内核模块</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>: $ modprobe overlay</t>
+    </r>
+  </si>
+  <si>
+    <t>overlayfs.md</t>
+  </si>
+  <si>
+    <t>overlayfs是目前使用比较广泛的层次文件系统，实现简单，性能较好</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>验证是否加载成功：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>lsmod |grep overlay</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>挂载</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>overlay</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>文件系统</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>将</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>low</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>和</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>upper</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>合并成一个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">merged </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>名称的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>overlayfs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>文件系统</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+ $ mount -t overlay overlay -olowerdir=./low,upperdir=./upper,workdir=./work ./merged</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>卸载</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>overlay</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>umount overlay</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">oprofile </t>
+  </si>
+  <si>
+    <t>1. install oprofile: yum install -y oprofile</t>
+  </si>
+  <si>
+    <t>oprofile.md</t>
+  </si>
+  <si>
+    <r>
+      <t>OProfile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Linux</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>内核支持的一种性能分析机制，是用于</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> Linux </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>评测和性能监控的工具</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>指示</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>oprofile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>启动检测后，不记录内核模块、内核代码相关统计数据：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>$ opcontrol --no-vmlinux</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>加载</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>oprofile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>模块、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>oprofile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>驱动程序：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>$ opcontrol --init</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>指示</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>oprofile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>启动检测：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">$ opcontrol --start </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>指示将</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>oprofile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>检测到的数据写入文件：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>$ opcontrol --dump</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">6. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>清空之前检测的数据记录：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>$ opcontrol --reset</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">7. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>关闭</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>oprofile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>进程：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>$ opcontrol -h</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">8. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>以镜像</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>(image)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的角度显示检测结果，进程、动态库、内核模块属于镜像范畴：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>$ opreport</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">9. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>以函数的角度显示检测结果：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>$ opreport -l</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>以函数的角度，针对</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>进程显示检测结果：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>$ opreport -l test</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">11. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>以代码的角度，针对</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>进程显示检测结果：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>$ opannotate -s test</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>12.remove oprofile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>yum remove -y oprofile</t>
+    </r>
   </si>
   <si>
     <t>lldptool</t>
   </si>
   <si>
     <t>1. install lldptool: yum install -y lldpad</t>
+  </si>
+  <si>
+    <t>lldptool.md</t>
   </si>
   <si>
     <t>2. Run the LLDP Daemon: lldpad -d</t>
@@ -3322,7 +4496,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -3492,6 +4666,37 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -3500,6 +4705,19 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -3519,10 +4737,10 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="thin">
         <color auto="1"/>
-      </right>
-      <top/>
+      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -3535,6 +4753,17 @@
       <right style="medium">
         <color auto="1"/>
       </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -3677,7 +4906,7 @@
     <xf numFmtId="0" fontId="35" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3717,32 +4946,32 @@
     <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="15" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
@@ -3752,7 +4981,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="19" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3773,16 +5002,16 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3971,7 +5200,22 @@
     <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="36" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="36" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="36" applyFont="1" applyBorder="1">
@@ -3980,35 +5224,67 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="36" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="44" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="44" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="44" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="36" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="36" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="16" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="36" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="36" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="36" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="36" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="176" fontId="14" fillId="4" borderId="11" xfId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="36" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -4030,19 +5306,43 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="36" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="36" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="36" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="16" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4467,18 +5767,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AMJ166"/>
+  <dimension ref="A1:AMJ196"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B154" sqref="B154"/>
+      <selection pane="bottomLeft" activeCell="D179" sqref="D179:D190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="17.0083333333333" style="33"/>
-    <col min="2" max="2" width="58.875" style="34" customWidth="1"/>
+    <col min="2" max="2" width="70.125" style="34" customWidth="1"/>
     <col min="3" max="3" width="6.475" style="34"/>
     <col min="4" max="4" width="19.0416666666667" style="33"/>
     <col min="5" max="5" width="8.775" style="35"/>
@@ -47090,437 +48390,950 @@
       <c r="D140" s="61" t="s">
         <v>182</v>
       </c>
-      <c r="E140" s="75" t="s">
+      <c r="E140" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="F140" s="76" t="s">
+      <c r="F140" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="G140" s="77"/>
-      <c r="H140" s="78"/>
-      <c r="I140" s="81"/>
+      <c r="G140" s="88"/>
+      <c r="H140" s="89"/>
+      <c r="I140" s="97"/>
     </row>
-    <row r="141" spans="1:9">
+    <row r="141" s="30" customFormat="1" ht="13" customHeight="1" spans="1:9">
       <c r="A141" s="62" t="s">
         <v>183</v>
       </c>
-      <c r="B141" s="63"/>
-      <c r="C141" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="D141" s="64"/>
-      <c r="E141" s="79"/>
-      <c r="F141" s="63"/>
-      <c r="G141" s="63"/>
-      <c r="H141" s="64"/>
-      <c r="I141" s="63"/>
+      <c r="B141" s="63" t="s">
+        <v>184</v>
+      </c>
+      <c r="C141" s="64"/>
+      <c r="D141" s="65"/>
+      <c r="E141" s="90"/>
+      <c r="F141" s="91"/>
+      <c r="G141" s="92"/>
+      <c r="H141" s="93"/>
+      <c r="I141" s="98" t="s">
+        <v>185</v>
+      </c>
     </row>
-    <row r="142" spans="1:9">
-      <c r="A142" s="65" t="s">
-        <v>184</v>
-      </c>
-      <c r="B142" s="66" t="s">
-        <v>185</v>
-      </c>
-      <c r="C142" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="D142" s="64"/>
-      <c r="E142" s="80" t="s">
-        <v>13</v>
-      </c>
-      <c r="F142" s="63"/>
-      <c r="G142" s="63"/>
-      <c r="H142" s="64"/>
-      <c r="I142" s="82" t="s">
-        <v>186</v>
-      </c>
+    <row r="142" s="30" customFormat="1" ht="13" customHeight="1" spans="1:9">
+      <c r="A142" s="66"/>
+      <c r="B142" s="63">
+        <v>2</v>
+      </c>
+      <c r="C142" s="64"/>
+      <c r="D142" s="65"/>
+      <c r="E142" s="90"/>
+      <c r="F142" s="91"/>
+      <c r="G142" s="92"/>
+      <c r="H142" s="93"/>
+      <c r="I142" s="98"/>
     </row>
-    <row r="143" spans="1:9">
-      <c r="A143" s="65"/>
-      <c r="B143" s="66" t="s">
-        <v>187</v>
-      </c>
-      <c r="C143" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="D143" s="64"/>
-      <c r="E143" s="80" t="s">
-        <v>13</v>
-      </c>
-      <c r="F143" s="63"/>
-      <c r="G143" s="63"/>
-      <c r="H143" s="64"/>
-      <c r="I143" s="83"/>
+    <row r="143" s="30" customFormat="1" ht="13" customHeight="1" spans="1:9">
+      <c r="A143" s="66"/>
+      <c r="B143" s="63"/>
+      <c r="C143" s="64"/>
+      <c r="D143" s="65"/>
+      <c r="E143" s="90"/>
+      <c r="F143" s="91"/>
+      <c r="G143" s="92"/>
+      <c r="H143" s="93"/>
+      <c r="I143" s="98"/>
     </row>
-    <row r="144" spans="1:9">
-      <c r="A144" s="65"/>
-      <c r="B144" s="66" t="s">
-        <v>188</v>
-      </c>
-      <c r="C144" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="D144" s="64"/>
-      <c r="E144" s="80" t="s">
-        <v>13</v>
-      </c>
-      <c r="F144" s="63"/>
-      <c r="G144" s="63"/>
-      <c r="H144" s="64"/>
-      <c r="I144" s="83"/>
+    <row r="144" s="30" customFormat="1" ht="13" customHeight="1" spans="1:9">
+      <c r="A144" s="66"/>
+      <c r="B144" s="63"/>
+      <c r="C144" s="64"/>
+      <c r="D144" s="65"/>
+      <c r="E144" s="90"/>
+      <c r="F144" s="91"/>
+      <c r="G144" s="92"/>
+      <c r="H144" s="93"/>
+      <c r="I144" s="98"/>
     </row>
-    <row r="145" spans="1:9">
-      <c r="A145" s="65"/>
-      <c r="B145" s="66" t="s">
-        <v>189</v>
-      </c>
-      <c r="C145" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="D145" s="64"/>
-      <c r="E145" s="80" t="s">
-        <v>13</v>
-      </c>
-      <c r="F145" s="63"/>
-      <c r="G145" s="63"/>
-      <c r="H145" s="64"/>
-      <c r="I145" s="83"/>
+    <row r="145" s="30" customFormat="1" ht="13" customHeight="1" spans="1:9">
+      <c r="A145" s="66"/>
+      <c r="B145" s="63"/>
+      <c r="C145" s="64"/>
+      <c r="D145" s="65"/>
+      <c r="E145" s="90"/>
+      <c r="F145" s="91"/>
+      <c r="G145" s="92"/>
+      <c r="H145" s="93"/>
+      <c r="I145" s="98"/>
     </row>
     <row r="146" spans="1:9">
-      <c r="A146" s="65"/>
-      <c r="B146" s="66" t="s">
-        <v>190</v>
-      </c>
+      <c r="A146" s="67"/>
+      <c r="B146" s="68"/>
       <c r="C146" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D146" s="64"/>
-      <c r="E146" s="80" t="s">
-        <v>13</v>
-      </c>
-      <c r="F146" s="63"/>
-      <c r="G146" s="63"/>
-      <c r="H146" s="64"/>
-      <c r="I146" s="83"/>
+      <c r="D146" s="69"/>
+      <c r="E146" s="94"/>
+      <c r="F146" s="68"/>
+      <c r="G146" s="68"/>
+      <c r="H146" s="69"/>
+      <c r="I146" s="68"/>
     </row>
     <row r="147" spans="1:9">
-      <c r="A147" s="65"/>
-      <c r="B147" s="66" t="s">
-        <v>191</v>
+      <c r="A147" s="70" t="s">
+        <v>186</v>
+      </c>
+      <c r="B147" s="71" t="s">
+        <v>187</v>
       </c>
       <c r="C147" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D147" s="64"/>
-      <c r="E147" s="80" t="s">
+      <c r="D147" s="72" t="s">
+        <v>188</v>
+      </c>
+      <c r="E147" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="F147" s="63"/>
-      <c r="G147" s="63"/>
-      <c r="H147" s="64"/>
-      <c r="I147" s="84"/>
+      <c r="F147" s="68"/>
+      <c r="G147" s="68"/>
+      <c r="H147" s="69"/>
+      <c r="I147" s="99" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="148" spans="1:9">
-      <c r="A148" s="67" t="s">
-        <v>192</v>
-      </c>
-      <c r="B148" s="68" t="s">
-        <v>193</v>
+      <c r="A148" s="70"/>
+      <c r="B148" s="71" t="s">
+        <v>190</v>
       </c>
       <c r="C148" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D148" s="64"/>
-      <c r="E148" s="80" t="s">
+      <c r="D148" s="73"/>
+      <c r="E148" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="F148" s="63"/>
-      <c r="G148" s="63"/>
-      <c r="H148" s="64"/>
-      <c r="I148" s="85" t="s">
-        <v>194</v>
-      </c>
+      <c r="F148" s="68"/>
+      <c r="G148" s="68"/>
+      <c r="H148" s="69"/>
+      <c r="I148" s="100"/>
     </row>
-    <row r="149" ht="82.5" spans="1:9">
-      <c r="A149" s="67"/>
-      <c r="B149" s="69" t="s">
-        <v>195</v>
+    <row r="149" spans="1:9">
+      <c r="A149" s="70"/>
+      <c r="B149" s="71" t="s">
+        <v>191</v>
       </c>
       <c r="C149" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D149" s="64"/>
-      <c r="E149" s="80" t="s">
+      <c r="D149" s="73"/>
+      <c r="E149" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="F149" s="63"/>
-      <c r="G149" s="63"/>
-      <c r="H149" s="64"/>
-      <c r="I149" s="83"/>
+      <c r="F149" s="68"/>
+      <c r="G149" s="68"/>
+      <c r="H149" s="69"/>
+      <c r="I149" s="100"/>
     </row>
     <row r="150" spans="1:9">
-      <c r="A150" s="70" t="s">
-        <v>196</v>
-      </c>
-      <c r="B150" s="63"/>
+      <c r="A150" s="70"/>
+      <c r="B150" s="71" t="s">
+        <v>192</v>
+      </c>
       <c r="C150" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D150" s="64"/>
-      <c r="E150" s="80" t="s">
+      <c r="D150" s="73"/>
+      <c r="E150" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="F150" s="63"/>
-      <c r="G150" s="63"/>
-      <c r="H150" s="64"/>
-      <c r="I150" s="63"/>
+      <c r="F150" s="68"/>
+      <c r="G150" s="68"/>
+      <c r="H150" s="69"/>
+      <c r="I150" s="100"/>
     </row>
     <row r="151" spans="1:9">
-      <c r="A151" s="71" t="s">
-        <v>197</v>
-      </c>
-      <c r="B151" s="63" t="s">
-        <v>198</v>
-      </c>
-      <c r="C151" s="40"/>
-      <c r="D151" s="64"/>
-      <c r="E151" s="80"/>
-      <c r="F151" s="63"/>
-      <c r="G151" s="63"/>
-      <c r="H151" s="64"/>
-      <c r="I151" s="63"/>
+      <c r="A151" s="70"/>
+      <c r="B151" s="71" t="s">
+        <v>193</v>
+      </c>
+      <c r="C151" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D151" s="73"/>
+      <c r="E151" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F151" s="68"/>
+      <c r="G151" s="68"/>
+      <c r="H151" s="69"/>
+      <c r="I151" s="100"/>
     </row>
     <row r="152" spans="1:9">
-      <c r="A152" s="65"/>
-      <c r="B152" s="63" t="s">
-        <v>199</v>
-      </c>
-      <c r="C152" s="40"/>
-      <c r="D152" s="64"/>
-      <c r="E152" s="80"/>
-      <c r="F152" s="63"/>
-      <c r="G152" s="63"/>
-      <c r="H152" s="64"/>
-      <c r="I152" s="63"/>
+      <c r="A152" s="70"/>
+      <c r="B152" s="71" t="s">
+        <v>194</v>
+      </c>
+      <c r="C152" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D152" s="74"/>
+      <c r="E152" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F152" s="68"/>
+      <c r="G152" s="68"/>
+      <c r="H152" s="69"/>
+      <c r="I152" s="101"/>
     </row>
     <row r="153" spans="1:9">
-      <c r="A153" s="65"/>
-      <c r="B153" s="63"/>
-      <c r="C153" s="40"/>
-      <c r="D153" s="64"/>
-      <c r="E153" s="80"/>
-      <c r="F153" s="63"/>
-      <c r="G153" s="63"/>
-      <c r="H153" s="64"/>
-      <c r="I153" s="63"/>
+      <c r="A153" s="75" t="s">
+        <v>195</v>
+      </c>
+      <c r="B153" s="76" t="s">
+        <v>196</v>
+      </c>
+      <c r="C153" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D153" s="72" t="s">
+        <v>197</v>
+      </c>
+      <c r="E153" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F153" s="68"/>
+      <c r="G153" s="68"/>
+      <c r="H153" s="69"/>
+      <c r="I153" s="102" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="154" spans="1:9">
-      <c r="A154" s="65"/>
-      <c r="B154" s="63"/>
-      <c r="C154" s="40"/>
-      <c r="D154" s="64"/>
-      <c r="E154" s="80"/>
-      <c r="F154" s="63"/>
-      <c r="G154" s="63"/>
-      <c r="H154" s="64"/>
-      <c r="I154" s="63"/>
+    <row r="154" ht="82.5" spans="1:9">
+      <c r="A154" s="75"/>
+      <c r="B154" s="77" t="s">
+        <v>199</v>
+      </c>
+      <c r="C154" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D154" s="74"/>
+      <c r="E154" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F154" s="68"/>
+      <c r="G154" s="68"/>
+      <c r="H154" s="69"/>
+      <c r="I154" s="100"/>
     </row>
     <row r="155" spans="1:9">
-      <c r="A155" s="65"/>
-      <c r="B155" s="63"/>
-      <c r="C155" s="40"/>
-      <c r="D155" s="64"/>
-      <c r="E155" s="80"/>
-      <c r="F155" s="63"/>
-      <c r="G155" s="63"/>
-      <c r="H155" s="64"/>
-      <c r="I155" s="63"/>
+      <c r="A155" s="70" t="s">
+        <v>200</v>
+      </c>
+      <c r="B155" s="78" t="s">
+        <v>201</v>
+      </c>
+      <c r="C155" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D155" s="72" t="s">
+        <v>202</v>
+      </c>
+      <c r="E155" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F155" s="68"/>
+      <c r="G155" s="68"/>
+      <c r="H155" s="69"/>
+      <c r="I155" s="100"/>
     </row>
     <row r="156" spans="1:9">
-      <c r="A156" s="65"/>
-      <c r="B156" s="63"/>
-      <c r="C156" s="40"/>
-      <c r="D156" s="64"/>
-      <c r="E156" s="80"/>
-      <c r="F156" s="63"/>
-      <c r="G156" s="63"/>
-      <c r="H156" s="64"/>
-      <c r="I156" s="63"/>
+      <c r="A156" s="70"/>
+      <c r="B156" s="78" t="s">
+        <v>203</v>
+      </c>
+      <c r="C156" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D156" s="73"/>
+      <c r="E156" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F156" s="68"/>
+      <c r="G156" s="68"/>
+      <c r="H156" s="69"/>
+      <c r="I156" s="100"/>
     </row>
     <row r="157" spans="1:9">
-      <c r="A157" s="72"/>
-      <c r="B157" s="63"/>
+      <c r="A157" s="70"/>
+      <c r="B157" s="68" t="s">
+        <v>204</v>
+      </c>
       <c r="C157" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D157" s="64"/>
-      <c r="E157" s="80" t="s">
+      <c r="D157" s="73"/>
+      <c r="E157" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="F157" s="63"/>
-      <c r="G157" s="63"/>
-      <c r="H157" s="64"/>
-      <c r="I157" s="63"/>
+      <c r="F157" s="68"/>
+      <c r="G157" s="68"/>
+      <c r="H157" s="69"/>
+      <c r="I157" s="100"/>
     </row>
     <row r="158" spans="1:9">
-      <c r="A158" s="62" t="s">
-        <v>200</v>
-      </c>
-      <c r="B158" s="63"/>
+      <c r="A158" s="70"/>
+      <c r="B158" s="68" t="s">
+        <v>205</v>
+      </c>
       <c r="C158" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D158" s="64"/>
-      <c r="E158" s="80" t="s">
+      <c r="D158" s="73"/>
+      <c r="E158" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="F158" s="63"/>
-      <c r="G158" s="63"/>
-      <c r="H158" s="64"/>
-      <c r="I158" s="63"/>
+      <c r="F158" s="68"/>
+      <c r="G158" s="68"/>
+      <c r="H158" s="69"/>
+      <c r="I158" s="100"/>
     </row>
     <row r="159" spans="1:9">
-      <c r="A159" s="62" t="s">
-        <v>201</v>
-      </c>
-      <c r="B159" s="63"/>
+      <c r="A159" s="70"/>
+      <c r="B159" s="68" t="s">
+        <v>206</v>
+      </c>
       <c r="C159" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D159" s="64"/>
-      <c r="E159" s="80" t="s">
+      <c r="D159" s="73"/>
+      <c r="E159" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="F159" s="63"/>
-      <c r="G159" s="63"/>
-      <c r="H159" s="64"/>
-      <c r="I159" s="63"/>
+      <c r="F159" s="68"/>
+      <c r="G159" s="68"/>
+      <c r="H159" s="69"/>
+      <c r="I159" s="100"/>
     </row>
     <row r="160" spans="1:9">
-      <c r="A160" s="62" t="s">
-        <v>202</v>
-      </c>
-      <c r="B160" s="63"/>
+      <c r="A160" s="70"/>
+      <c r="B160" s="78" t="s">
+        <v>207</v>
+      </c>
       <c r="C160" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D160" s="64"/>
-      <c r="E160" s="80" t="s">
+      <c r="D160" s="73"/>
+      <c r="E160" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="F160" s="63"/>
-      <c r="G160" s="63"/>
-      <c r="H160" s="64"/>
-      <c r="I160" s="63"/>
+      <c r="F160" s="68"/>
+      <c r="G160" s="68"/>
+      <c r="H160" s="69"/>
+      <c r="I160" s="100"/>
     </row>
     <row r="161" spans="1:9">
-      <c r="A161" s="71" t="s">
-        <v>203</v>
-      </c>
-      <c r="B161" s="63" t="s">
-        <v>204</v>
+      <c r="A161" s="70"/>
+      <c r="B161" s="78" t="s">
+        <v>208</v>
       </c>
       <c r="C161" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D161" s="64"/>
-      <c r="E161" s="80" t="s">
+      <c r="D161" s="73"/>
+      <c r="E161" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="F161" s="63"/>
-      <c r="G161" s="63"/>
-      <c r="H161" s="64"/>
-      <c r="I161" s="63"/>
+      <c r="F161" s="68"/>
+      <c r="G161" s="68"/>
+      <c r="H161" s="69"/>
+      <c r="I161" s="100"/>
     </row>
     <row r="162" spans="1:9">
-      <c r="A162" s="65"/>
-      <c r="B162" s="63" t="s">
-        <v>205</v>
+      <c r="A162" s="79"/>
+      <c r="B162" s="68" t="s">
+        <v>209</v>
       </c>
       <c r="C162" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D162" s="64"/>
-      <c r="E162" s="80" t="s">
+      <c r="D162" s="74"/>
+      <c r="E162" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="F162" s="63"/>
-      <c r="G162" s="63"/>
-      <c r="H162" s="64"/>
-      <c r="I162" s="63"/>
+      <c r="F162" s="68"/>
+      <c r="G162" s="68"/>
+      <c r="H162" s="69"/>
+      <c r="I162" s="68"/>
     </row>
-    <row r="163" ht="112.5" spans="1:9">
-      <c r="A163" s="65"/>
-      <c r="B163" s="73" t="s">
-        <v>206</v>
-      </c>
-      <c r="C163" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="D163" s="64"/>
-      <c r="E163" s="80" t="s">
-        <v>13</v>
-      </c>
-      <c r="F163" s="63"/>
-      <c r="G163" s="63"/>
-      <c r="H163" s="64"/>
-      <c r="I163" s="63"/>
+    <row r="163" spans="1:9">
+      <c r="A163" s="80" t="s">
+        <v>210</v>
+      </c>
+      <c r="B163" s="68" t="s">
+        <v>211</v>
+      </c>
+      <c r="C163" s="40"/>
+      <c r="D163" s="69"/>
+      <c r="E163" s="95"/>
+      <c r="F163" s="68"/>
+      <c r="G163" s="68"/>
+      <c r="H163" s="69"/>
+      <c r="I163" s="103" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="164" spans="1:9">
-      <c r="A164" s="65"/>
-      <c r="B164" s="63" t="s">
-        <v>207</v>
-      </c>
-      <c r="C164" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="D164" s="64"/>
-      <c r="E164" s="80" t="s">
-        <v>13</v>
-      </c>
-      <c r="F164" s="63"/>
-      <c r="G164" s="63"/>
-      <c r="H164" s="64"/>
-      <c r="I164" s="63"/>
+      <c r="A164" s="70"/>
+      <c r="B164" s="68" t="s">
+        <v>213</v>
+      </c>
+      <c r="C164" s="40"/>
+      <c r="D164" s="69"/>
+      <c r="E164" s="95"/>
+      <c r="F164" s="68"/>
+      <c r="G164" s="68"/>
+      <c r="H164" s="69"/>
+      <c r="I164" s="102"/>
     </row>
     <row r="165" spans="1:9">
-      <c r="A165" s="74"/>
-      <c r="B165" s="63" t="s">
-        <v>208</v>
-      </c>
-      <c r="C165" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="D165" s="64"/>
-      <c r="E165" s="80" t="s">
-        <v>13</v>
-      </c>
-      <c r="F165" s="63"/>
-      <c r="G165" s="63"/>
-      <c r="H165" s="64"/>
-      <c r="I165" s="63"/>
+      <c r="A165" s="70"/>
+      <c r="C165" s="40"/>
+      <c r="D165" s="69"/>
+      <c r="E165" s="95"/>
+      <c r="F165" s="68"/>
+      <c r="G165" s="68"/>
+      <c r="H165" s="69"/>
+      <c r="I165" s="102"/>
     </row>
     <row r="166" spans="1:9">
-      <c r="A166" s="62" t="s">
-        <v>209</v>
-      </c>
-      <c r="B166" s="63"/>
-      <c r="C166" s="40" t="s">
+      <c r="A166" s="70"/>
+      <c r="C166" s="40"/>
+      <c r="D166" s="69"/>
+      <c r="E166" s="95"/>
+      <c r="F166" s="68"/>
+      <c r="G166" s="68"/>
+      <c r="H166" s="69"/>
+      <c r="I166" s="102"/>
+    </row>
+    <row r="167" spans="1:9">
+      <c r="A167" s="70"/>
+      <c r="C167" s="40"/>
+      <c r="D167" s="69"/>
+      <c r="E167" s="95"/>
+      <c r="F167" s="68"/>
+      <c r="G167" s="68"/>
+      <c r="H167" s="69"/>
+      <c r="I167" s="102"/>
+    </row>
+    <row r="168" spans="1:9">
+      <c r="A168" s="70"/>
+      <c r="B168" s="68"/>
+      <c r="C168" s="40"/>
+      <c r="D168" s="69"/>
+      <c r="E168" s="95"/>
+      <c r="F168" s="68"/>
+      <c r="G168" s="68"/>
+      <c r="H168" s="69"/>
+      <c r="I168" s="102"/>
+    </row>
+    <row r="169" spans="1:9">
+      <c r="A169" s="79"/>
+      <c r="B169" s="68"/>
+      <c r="C169" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D166" s="64"/>
-      <c r="E166" s="80" t="s">
+      <c r="D169" s="69"/>
+      <c r="E169" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="F166" s="63"/>
-      <c r="G166" s="63"/>
-      <c r="H166" s="64"/>
-      <c r="I166" s="63"/>
+      <c r="F169" s="68"/>
+      <c r="G169" s="68"/>
+      <c r="H169" s="69"/>
+      <c r="I169" s="104"/>
+    </row>
+    <row r="170" spans="1:9">
+      <c r="A170" s="70" t="s">
+        <v>214</v>
+      </c>
+      <c r="B170" s="68" t="s">
+        <v>215</v>
+      </c>
+      <c r="C170" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D170" s="72" t="s">
+        <v>216</v>
+      </c>
+      <c r="E170" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F170" s="68"/>
+      <c r="G170" s="68"/>
+      <c r="H170" s="69"/>
+      <c r="I170" s="102" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9">
+      <c r="A171" s="70"/>
+      <c r="B171" s="68" t="s">
+        <v>218</v>
+      </c>
+      <c r="C171" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D171" s="73"/>
+      <c r="E171" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F171" s="68"/>
+      <c r="G171" s="68"/>
+      <c r="H171" s="69"/>
+      <c r="I171" s="102"/>
+    </row>
+    <row r="172" ht="159.75" spans="1:9">
+      <c r="A172" s="70"/>
+      <c r="B172" s="81" t="s">
+        <v>219</v>
+      </c>
+      <c r="C172" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D172" s="73"/>
+      <c r="E172" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F172" s="68"/>
+      <c r="G172" s="68"/>
+      <c r="H172" s="69"/>
+      <c r="I172" s="102"/>
+    </row>
+    <row r="173" ht="229.5" spans="1:9">
+      <c r="A173" s="70"/>
+      <c r="B173" s="81" t="s">
+        <v>220</v>
+      </c>
+      <c r="C173" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D173" s="73"/>
+      <c r="E173" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F173" s="68"/>
+      <c r="G173" s="68"/>
+      <c r="H173" s="69"/>
+      <c r="I173" s="104"/>
+    </row>
+    <row r="174" spans="1:9">
+      <c r="A174" s="70"/>
+      <c r="B174" s="82" t="s">
+        <v>221</v>
+      </c>
+      <c r="C174" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D174" s="74"/>
+      <c r="E174" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F174" s="68"/>
+      <c r="G174" s="68"/>
+      <c r="H174" s="69"/>
+      <c r="I174" s="102"/>
+    </row>
+    <row r="175" spans="1:9">
+      <c r="A175" s="80" t="s">
+        <v>222</v>
+      </c>
+      <c r="B175" s="83" t="s">
+        <v>223</v>
+      </c>
+      <c r="C175" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D175" s="72" t="s">
+        <v>224</v>
+      </c>
+      <c r="E175" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F175" s="68"/>
+      <c r="G175" s="68"/>
+      <c r="H175" s="96"/>
+      <c r="I175" s="105" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9">
+      <c r="A176" s="70"/>
+      <c r="B176" s="83" t="s">
+        <v>226</v>
+      </c>
+      <c r="C176" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D176" s="73"/>
+      <c r="E176" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F176" s="68"/>
+      <c r="G176" s="68"/>
+      <c r="H176" s="96"/>
+      <c r="I176" s="105"/>
+    </row>
+    <row r="177" ht="22.5" spans="1:9">
+      <c r="A177" s="70"/>
+      <c r="B177" s="84" t="s">
+        <v>227</v>
+      </c>
+      <c r="C177" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D177" s="73"/>
+      <c r="E177" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F177" s="68"/>
+      <c r="G177" s="68"/>
+      <c r="H177" s="96"/>
+      <c r="I177" s="105"/>
+    </row>
+    <row r="178" spans="1:9">
+      <c r="A178" s="79"/>
+      <c r="B178" s="83" t="s">
+        <v>228</v>
+      </c>
+      <c r="C178" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D178" s="74"/>
+      <c r="E178" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F178" s="68"/>
+      <c r="G178" s="68"/>
+      <c r="H178" s="96"/>
+      <c r="I178" s="105"/>
+    </row>
+    <row r="179" spans="1:9">
+      <c r="A179" s="70" t="s">
+        <v>229</v>
+      </c>
+      <c r="B179" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="C179" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D179" s="72" t="s">
+        <v>231</v>
+      </c>
+      <c r="E179" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F179" s="68"/>
+      <c r="G179" s="68"/>
+      <c r="H179" s="69"/>
+      <c r="I179" s="106" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9">
+      <c r="A180" s="70"/>
+      <c r="B180" s="84" t="s">
+        <v>233</v>
+      </c>
+      <c r="C180" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D180" s="73"/>
+      <c r="E180" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F180" s="68"/>
+      <c r="G180" s="68"/>
+      <c r="H180" s="69"/>
+      <c r="I180" s="100"/>
+    </row>
+    <row r="181" spans="1:9">
+      <c r="A181" s="70"/>
+      <c r="B181" s="84" t="s">
+        <v>234</v>
+      </c>
+      <c r="C181" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D181" s="73"/>
+      <c r="E181" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F181" s="68"/>
+      <c r="G181" s="68"/>
+      <c r="H181" s="69"/>
+      <c r="I181" s="100"/>
+    </row>
+    <row r="182" spans="1:9">
+      <c r="A182" s="70"/>
+      <c r="B182" s="83" t="s">
+        <v>235</v>
+      </c>
+      <c r="C182" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D182" s="73"/>
+      <c r="E182" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F182" s="68"/>
+      <c r="G182" s="68"/>
+      <c r="H182" s="69"/>
+      <c r="I182" s="100"/>
+    </row>
+    <row r="183" spans="1:9">
+      <c r="A183" s="70"/>
+      <c r="B183" s="85" t="s">
+        <v>236</v>
+      </c>
+      <c r="C183" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D183" s="73"/>
+      <c r="E183" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F183" s="68"/>
+      <c r="G183" s="68"/>
+      <c r="H183" s="69"/>
+      <c r="I183" s="100"/>
+    </row>
+    <row r="184" spans="1:9">
+      <c r="A184" s="70"/>
+      <c r="B184" s="85" t="s">
+        <v>237</v>
+      </c>
+      <c r="C184" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D184" s="73"/>
+      <c r="E184" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F184" s="68"/>
+      <c r="G184" s="68"/>
+      <c r="H184" s="69"/>
+      <c r="I184" s="100"/>
+    </row>
+    <row r="185" spans="1:9">
+      <c r="A185" s="70"/>
+      <c r="B185" s="85" t="s">
+        <v>238</v>
+      </c>
+      <c r="C185" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D185" s="73"/>
+      <c r="E185" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F185" s="68"/>
+      <c r="G185" s="68"/>
+      <c r="H185" s="69"/>
+      <c r="I185" s="100"/>
+    </row>
+    <row r="186" spans="1:9">
+      <c r="A186" s="70"/>
+      <c r="B186" s="82" t="s">
+        <v>239</v>
+      </c>
+      <c r="C186" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D186" s="73"/>
+      <c r="E186" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F186" s="68"/>
+      <c r="G186" s="68"/>
+      <c r="H186" s="69"/>
+      <c r="I186" s="100"/>
+    </row>
+    <row r="187" spans="1:9">
+      <c r="A187" s="70"/>
+      <c r="B187" s="85" t="s">
+        <v>240</v>
+      </c>
+      <c r="C187" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D187" s="73"/>
+      <c r="E187" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F187" s="68"/>
+      <c r="G187" s="68"/>
+      <c r="H187" s="69"/>
+      <c r="I187" s="100"/>
+    </row>
+    <row r="188" spans="1:9">
+      <c r="A188" s="70"/>
+      <c r="B188" s="85" t="s">
+        <v>241</v>
+      </c>
+      <c r="C188" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D188" s="73"/>
+      <c r="E188" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F188" s="68"/>
+      <c r="G188" s="68"/>
+      <c r="H188" s="69"/>
+      <c r="I188" s="100"/>
+    </row>
+    <row r="189" spans="1:9">
+      <c r="A189" s="70"/>
+      <c r="B189" s="85" t="s">
+        <v>242</v>
+      </c>
+      <c r="C189" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D189" s="73"/>
+      <c r="E189" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F189" s="68"/>
+      <c r="G189" s="68"/>
+      <c r="H189" s="69"/>
+      <c r="I189" s="100"/>
+    </row>
+    <row r="190" spans="1:9">
+      <c r="A190" s="70"/>
+      <c r="B190" s="85" t="s">
+        <v>243</v>
+      </c>
+      <c r="C190" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D190" s="74"/>
+      <c r="E190" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F190" s="68"/>
+      <c r="G190" s="68"/>
+      <c r="H190" s="69"/>
+      <c r="I190" s="101"/>
+    </row>
+    <row r="191" spans="1:9">
+      <c r="A191" s="80" t="s">
+        <v>244</v>
+      </c>
+      <c r="B191" s="68" t="s">
+        <v>245</v>
+      </c>
+      <c r="C191" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D191" s="72" t="s">
+        <v>246</v>
+      </c>
+      <c r="E191" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F191" s="68"/>
+      <c r="G191" s="68"/>
+      <c r="H191" s="69"/>
+      <c r="I191" s="99"/>
+    </row>
+    <row r="192" spans="1:9">
+      <c r="A192" s="70"/>
+      <c r="B192" s="68" t="s">
+        <v>247</v>
+      </c>
+      <c r="C192" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D192" s="73"/>
+      <c r="E192" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F192" s="68"/>
+      <c r="G192" s="68"/>
+      <c r="H192" s="69"/>
+      <c r="I192" s="100"/>
+    </row>
+    <row r="193" ht="112.5" spans="1:9">
+      <c r="A193" s="70"/>
+      <c r="B193" s="81" t="s">
+        <v>248</v>
+      </c>
+      <c r="C193" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D193" s="73"/>
+      <c r="E193" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F193" s="68"/>
+      <c r="G193" s="68"/>
+      <c r="H193" s="69"/>
+      <c r="I193" s="100"/>
+    </row>
+    <row r="194" spans="1:9">
+      <c r="A194" s="70"/>
+      <c r="B194" s="68" t="s">
+        <v>249</v>
+      </c>
+      <c r="C194" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D194" s="73"/>
+      <c r="E194" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F194" s="68"/>
+      <c r="G194" s="68"/>
+      <c r="H194" s="69"/>
+      <c r="I194" s="100"/>
+    </row>
+    <row r="195" spans="1:9">
+      <c r="A195" s="107"/>
+      <c r="B195" s="68" t="s">
+        <v>250</v>
+      </c>
+      <c r="C195" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D195" s="74"/>
+      <c r="E195" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F195" s="68"/>
+      <c r="G195" s="68"/>
+      <c r="H195" s="69"/>
+      <c r="I195" s="101"/>
+    </row>
+    <row r="196" spans="1:9">
+      <c r="A196" s="108" t="s">
+        <v>251</v>
+      </c>
+      <c r="B196" s="68"/>
+      <c r="C196" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D196" s="69"/>
+      <c r="E196" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F196" s="68"/>
+      <c r="G196" s="68"/>
+      <c r="H196" s="69"/>
+      <c r="I196" s="68"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I166"/>
-  <mergeCells count="30">
+  <autoFilter ref="A1:I196"/>
+  <mergeCells count="47">
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="A10:A22"/>
     <mergeCell ref="A23:A34"/>
@@ -47533,10 +49346,15 @@
     <mergeCell ref="A106:A119"/>
     <mergeCell ref="A120:A123"/>
     <mergeCell ref="A124:A139"/>
-    <mergeCell ref="A142:A147"/>
-    <mergeCell ref="A148:A149"/>
-    <mergeCell ref="A151:A157"/>
-    <mergeCell ref="A161:A165"/>
+    <mergeCell ref="A141:A146"/>
+    <mergeCell ref="A147:A152"/>
+    <mergeCell ref="A153:A154"/>
+    <mergeCell ref="A155:A162"/>
+    <mergeCell ref="A163:A169"/>
+    <mergeCell ref="A170:A173"/>
+    <mergeCell ref="A175:A178"/>
+    <mergeCell ref="A179:A190"/>
+    <mergeCell ref="A191:A195"/>
     <mergeCell ref="D2:D9"/>
     <mergeCell ref="D10:D22"/>
     <mergeCell ref="D23:D34"/>
@@ -47549,10 +49367,22 @@
     <mergeCell ref="D106:D119"/>
     <mergeCell ref="D120:D123"/>
     <mergeCell ref="D124:D139"/>
-    <mergeCell ref="I142:I147"/>
-    <mergeCell ref="I148:I149"/>
+    <mergeCell ref="D147:D152"/>
+    <mergeCell ref="D153:D154"/>
+    <mergeCell ref="D155:D162"/>
+    <mergeCell ref="D170:D174"/>
+    <mergeCell ref="D175:D178"/>
+    <mergeCell ref="D179:D190"/>
+    <mergeCell ref="D191:D195"/>
+    <mergeCell ref="I147:I152"/>
+    <mergeCell ref="I153:I154"/>
+    <mergeCell ref="I163:I169"/>
+    <mergeCell ref="I170:I173"/>
+    <mergeCell ref="I175:I178"/>
+    <mergeCell ref="I179:I190"/>
+    <mergeCell ref="I191:I195"/>
   </mergeCells>
-  <conditionalFormatting sqref="G2:G140">
+  <conditionalFormatting sqref="G2:G145">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -47561,11 +49391,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="H2 H3 H140 H4:H9 H23:H85 H101:H119 H120:H139"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2 G3 G140 G4:G119 G120:G139">
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="H2 H3 H140 H4:H9 H23:H85 H101:H119 H120:H139 H141:H145"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2 G3 G140 G4:G119 G120:G139 G141:G145">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="PLS Select 请选择" sqref="F2 F3 F140 F4:F119 F120:F139">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="PLS Select 请选择" sqref="F2 F3 F140 F4:F119 F120:F139 F141:F145">
       <formula1>"是,否"</formula1>
     </dataValidation>
   </dataValidations>
@@ -47596,6 +49426,13 @@
     <hyperlink ref="D106:D119" r:id="rId24" display="lttng-modules.sh"/>
     <hyperlink ref="D120:D123" r:id="rId25" display="grafana.sh"/>
     <hyperlink ref="D124:D139" r:id="rId26" display="ktap.md"/>
+    <hyperlink ref="D153:D154" r:id="rId26" display="setpci.md"/>
+    <hyperlink ref="D155:D162" r:id="rId27" display="swapon.sh"/>
+    <hyperlink ref="D170:D174" r:id="rId28" display="valgrind.md"/>
+    <hyperlink ref="D175:D178" r:id="rId29" display="overlayfs.md"/>
+    <hyperlink ref="D179:D190" r:id="rId30" display="oprofile.md"/>
+    <hyperlink ref="D191:D195" r:id="rId31" display="lldptool.md"/>
+    <hyperlink ref="D147:D152" r:id="rId32" display="pidstat.sh"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -47659,16 +49496,16 @@
     </row>
     <row r="2" customFormat="1" ht="13.5" customHeight="1" spans="1:9">
       <c r="A2" s="6" t="s">
-        <v>210</v>
+        <v>252</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>158</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>212</v>
+        <v>254</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>13</v>
@@ -47690,7 +49527,7 @@
         <v>160</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="14" t="s">
@@ -47713,7 +49550,7 @@
         <v>161</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="14" t="s">
@@ -47736,7 +49573,7 @@
         <v>162</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="14" t="s">
@@ -47755,16 +49592,16 @@
     </row>
     <row r="6" customFormat="1" ht="13.5" customHeight="1" spans="1:9">
       <c r="A6" s="6" t="s">
-        <v>213</v>
+        <v>255</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>158</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>214</v>
+        <v>256</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>13</v>
@@ -47786,7 +49623,7 @@
         <v>160</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="14" t="s">
@@ -47809,7 +49646,7 @@
         <v>161</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="14" t="s">
@@ -47832,7 +49669,7 @@
         <v>162</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="14" t="s">
@@ -47851,16 +49688,16 @@
     </row>
     <row r="10" ht="13.5" customHeight="1" spans="1:9">
       <c r="A10" s="6" t="s">
-        <v>215</v>
+        <v>257</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>158</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>216</v>
+        <v>258</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>13</v>
@@ -47882,7 +49719,7 @@
         <v>160</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="14" t="s">
@@ -47905,7 +49742,7 @@
         <v>161</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="14" t="s">
@@ -47928,7 +49765,7 @@
         <v>162</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="14" t="s">
@@ -47947,16 +49784,16 @@
     </row>
     <row r="14" ht="13.5" customHeight="1" spans="1:9">
       <c r="A14" s="6" t="s">
-        <v>217</v>
+        <v>259</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>158</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>218</v>
+        <v>260</v>
       </c>
       <c r="E14" s="14" t="s">
         <v>13</v>
@@ -47978,7 +49815,7 @@
         <v>160</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="14" t="s">
@@ -48001,7 +49838,7 @@
         <v>161</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="14" t="s">
@@ -48024,7 +49861,7 @@
         <v>162</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="14" t="s">
@@ -48043,16 +49880,16 @@
     </row>
     <row r="18" ht="13.5" customHeight="1" spans="1:9">
       <c r="A18" s="6" t="s">
-        <v>219</v>
+        <v>261</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>158</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>13</v>
@@ -48074,7 +49911,7 @@
         <v>160</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D19" s="13"/>
       <c r="E19" s="14" t="s">
@@ -48097,7 +49934,7 @@
         <v>161</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="14" t="s">
@@ -48120,7 +49957,7 @@
         <v>162</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="14" t="s">
@@ -48139,16 +49976,16 @@
     </row>
     <row r="22" ht="13.5" customHeight="1" spans="1:9">
       <c r="A22" s="6" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>158</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>222</v>
+        <v>264</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>13</v>
@@ -48170,7 +50007,7 @@
         <v>160</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="14" t="s">
@@ -48193,7 +50030,7 @@
         <v>161</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D24" s="13"/>
       <c r="E24" s="14" t="s">
@@ -48216,7 +50053,7 @@
         <v>162</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D25" s="13"/>
       <c r="E25" s="14" t="s">
@@ -48235,16 +50072,16 @@
     </row>
     <row r="26" ht="13.5" customHeight="1" spans="1:9">
       <c r="A26" s="6" t="s">
-        <v>223</v>
+        <v>265</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>158</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>224</v>
+        <v>266</v>
       </c>
       <c r="E26" s="14" t="s">
         <v>13</v>
@@ -48266,7 +50103,7 @@
         <v>160</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D27" s="13"/>
       <c r="E27" s="14" t="s">
@@ -48289,7 +50126,7 @@
         <v>161</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D28" s="13"/>
       <c r="E28" s="14" t="s">
@@ -48312,7 +50149,7 @@
         <v>162</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D29" s="13"/>
       <c r="E29" s="14" t="s">
@@ -48331,16 +50168,16 @@
     </row>
     <row r="30" ht="13.5" customHeight="1" spans="1:9">
       <c r="A30" s="6" t="s">
-        <v>225</v>
+        <v>267</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>158</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>226</v>
+        <v>268</v>
       </c>
       <c r="E30" s="14" t="s">
         <v>13</v>
@@ -48362,7 +50199,7 @@
         <v>160</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D31" s="13"/>
       <c r="E31" s="14" t="s">
@@ -48385,7 +50222,7 @@
         <v>161</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D32" s="13"/>
       <c r="E32" s="14" t="s">
@@ -48408,7 +50245,7 @@
         <v>162</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D33" s="13"/>
       <c r="E33" s="14" t="s">
@@ -48427,16 +50264,16 @@
     </row>
     <row r="34" ht="13.5" customHeight="1" spans="1:9">
       <c r="A34" s="6" t="s">
-        <v>227</v>
+        <v>269</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>158</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>228</v>
+        <v>270</v>
       </c>
       <c r="E34" s="14" t="s">
         <v>13</v>
@@ -48458,7 +50295,7 @@
         <v>160</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D35" s="13"/>
       <c r="E35" s="14" t="s">
@@ -48481,7 +50318,7 @@
         <v>161</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D36" s="13"/>
       <c r="E36" s="14" t="s">
@@ -48504,7 +50341,7 @@
         <v>162</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D37" s="13"/>
       <c r="E37" s="14" t="s">
@@ -48523,16 +50360,16 @@
     </row>
     <row r="38" ht="13.5" customHeight="1" spans="1:9">
       <c r="A38" s="6" t="s">
-        <v>229</v>
+        <v>271</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>158</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>230</v>
+        <v>272</v>
       </c>
       <c r="E38" s="14" t="s">
         <v>13</v>
@@ -48554,7 +50391,7 @@
         <v>160</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="14" t="s">
@@ -48577,7 +50414,7 @@
         <v>161</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="14" t="s">
@@ -48600,7 +50437,7 @@
         <v>162</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="14" t="s">
@@ -48619,16 +50456,16 @@
     </row>
     <row r="42" ht="13.5" customHeight="1" spans="1:9">
       <c r="A42" s="6" t="s">
-        <v>231</v>
+        <v>273</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>158</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>232</v>
+        <v>274</v>
       </c>
       <c r="E42" s="14" t="s">
         <v>13</v>
@@ -48650,7 +50487,7 @@
         <v>160</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D43" s="13"/>
       <c r="E43" s="14" t="s">
@@ -48673,7 +50510,7 @@
         <v>161</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D44" s="13"/>
       <c r="E44" s="14" t="s">
@@ -48696,7 +50533,7 @@
         <v>162</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D45" s="13"/>
       <c r="E45" s="14" t="s">
@@ -48715,16 +50552,16 @@
     </row>
     <row r="46" ht="13.5" customHeight="1" spans="1:9">
       <c r="A46" s="6" t="s">
-        <v>233</v>
+        <v>275</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>158</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>234</v>
+        <v>276</v>
       </c>
       <c r="E46" s="14" t="s">
         <v>13</v>
@@ -48746,7 +50583,7 @@
         <v>160</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D47" s="13"/>
       <c r="E47" s="14" t="s">
@@ -48769,7 +50606,7 @@
         <v>161</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D48" s="13"/>
       <c r="E48" s="14" t="s">
@@ -48792,7 +50629,7 @@
         <v>162</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D49" s="13"/>
       <c r="E49" s="14" t="s">
@@ -48811,16 +50648,16 @@
     </row>
     <row r="50" ht="13.5" customHeight="1" spans="1:9">
       <c r="A50" s="6" t="s">
-        <v>235</v>
+        <v>277</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>158</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>236</v>
+        <v>278</v>
       </c>
       <c r="E50" s="14" t="s">
         <v>13</v>
@@ -48842,7 +50679,7 @@
         <v>160</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D51" s="13"/>
       <c r="E51" s="14" t="s">
@@ -48865,7 +50702,7 @@
         <v>161</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D52" s="13"/>
       <c r="E52" s="14" t="s">
@@ -48888,7 +50725,7 @@
         <v>162</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D53" s="13"/>
       <c r="E53" s="14" t="s">
@@ -48907,16 +50744,16 @@
     </row>
     <row r="54" ht="13.5" customHeight="1" spans="1:9">
       <c r="A54" s="6" t="s">
-        <v>237</v>
+        <v>279</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>158</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>238</v>
+        <v>280</v>
       </c>
       <c r="E54" s="14" t="s">
         <v>13</v>
@@ -48938,7 +50775,7 @@
         <v>160</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D55" s="13"/>
       <c r="E55" s="14" t="s">
@@ -48961,7 +50798,7 @@
         <v>161</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D56" s="13"/>
       <c r="E56" s="14" t="s">
@@ -48984,7 +50821,7 @@
         <v>162</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D57" s="13"/>
       <c r="E57" s="14" t="s">
@@ -49003,16 +50840,16 @@
     </row>
     <row r="58" ht="13.5" customHeight="1" spans="1:9">
       <c r="A58" s="6" t="s">
-        <v>239</v>
+        <v>281</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>158</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>240</v>
+        <v>282</v>
       </c>
       <c r="E58" s="14" t="s">
         <v>13</v>
@@ -49034,7 +50871,7 @@
         <v>160</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D59" s="13"/>
       <c r="E59" s="14" t="s">
@@ -49057,7 +50894,7 @@
         <v>161</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D60" s="13"/>
       <c r="E60" s="14" t="s">
@@ -49080,7 +50917,7 @@
         <v>162</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D61" s="13"/>
       <c r="E61" s="14" t="s">
@@ -49099,16 +50936,16 @@
     </row>
     <row r="62" s="1" customFormat="1" ht="13.5" customHeight="1" spans="1:9">
       <c r="A62" s="6" t="s">
-        <v>241</v>
+        <v>283</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>242</v>
+        <v>284</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>243</v>
+        <v>285</v>
       </c>
       <c r="E62" s="14" t="s">
         <v>13</v>
@@ -49130,7 +50967,7 @@
         <v>160</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D63" s="13"/>
       <c r="E63" s="14" t="s">
@@ -49153,7 +50990,7 @@
         <v>161</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D64" s="13"/>
       <c r="E64" s="14" t="s">
@@ -49173,10 +51010,10 @@
     <row r="65" spans="1:9">
       <c r="A65" s="6"/>
       <c r="B65" s="11" t="s">
-        <v>244</v>
+        <v>286</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D65" s="13"/>
       <c r="E65" s="14" t="s">
@@ -49196,10 +51033,10 @@
     <row r="66" spans="1:9">
       <c r="A66" s="6"/>
       <c r="B66" s="11" t="s">
-        <v>245</v>
+        <v>287</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D66" s="13"/>
       <c r="E66" s="14" t="s">
@@ -49219,10 +51056,10 @@
     <row r="67" spans="1:9">
       <c r="A67" s="6"/>
       <c r="B67" s="11" t="s">
-        <v>246</v>
+        <v>288</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D67" s="13"/>
       <c r="E67" s="14" t="s">
@@ -49242,10 +51079,10 @@
     <row r="68" spans="1:9">
       <c r="A68" s="6"/>
       <c r="B68" s="11" t="s">
-        <v>247</v>
+        <v>289</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D68" s="13"/>
       <c r="E68" s="14" t="s">
@@ -49265,10 +51102,10 @@
     <row r="69" spans="1:9">
       <c r="A69" s="6"/>
       <c r="B69" s="11" t="s">
-        <v>248</v>
+        <v>290</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D69" s="13"/>
       <c r="E69" s="14" t="s">
@@ -49288,10 +51125,10 @@
     <row r="70" spans="1:9">
       <c r="A70" s="6"/>
       <c r="B70" s="11" t="s">
-        <v>249</v>
+        <v>291</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D70" s="13"/>
       <c r="E70" s="14" t="s">
@@ -49311,10 +51148,10 @@
     <row r="71" spans="1:9">
       <c r="A71" s="6"/>
       <c r="B71" s="11" t="s">
-        <v>250</v>
+        <v>292</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D71" s="13"/>
       <c r="E71" s="14" t="s">
@@ -49334,10 +51171,10 @@
     <row r="72" spans="1:9">
       <c r="A72" s="6"/>
       <c r="B72" s="11" t="s">
-        <v>251</v>
+        <v>293</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D72" s="13"/>
       <c r="E72" s="14" t="s">
@@ -49356,16 +51193,16 @@
     </row>
     <row r="73" customFormat="1" ht="13.5" customHeight="1" spans="1:9">
       <c r="A73" s="6" t="s">
-        <v>252</v>
+        <v>294</v>
       </c>
       <c r="B73" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="C73" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="C73" s="21" t="s">
-        <v>211</v>
-      </c>
       <c r="D73" s="13" t="s">
-        <v>254</v>
+        <v>296</v>
       </c>
       <c r="E73" s="14" t="s">
         <v>13</v>
@@ -49387,7 +51224,7 @@
         <v>160</v>
       </c>
       <c r="C74" s="21" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D74" s="13"/>
       <c r="E74" s="14" t="s">
@@ -49410,7 +51247,7 @@
         <v>161</v>
       </c>
       <c r="C75" s="21" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D75" s="13"/>
       <c r="E75" s="14" t="s">
@@ -49430,10 +51267,10 @@
     <row r="76" customFormat="1" ht="13.5" spans="1:9">
       <c r="A76" s="6"/>
       <c r="B76" s="20" t="s">
-        <v>255</v>
+        <v>297</v>
       </c>
       <c r="C76" s="21" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D76" s="13"/>
       <c r="E76" s="14" t="s">
@@ -49453,10 +51290,10 @@
     <row r="77" customFormat="1" ht="13.5" spans="1:9">
       <c r="A77" s="6"/>
       <c r="B77" s="20" t="s">
-        <v>256</v>
+        <v>298</v>
       </c>
       <c r="C77" s="21" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D77" s="13"/>
       <c r="E77" s="14" t="s">
@@ -49476,10 +51313,10 @@
     <row r="78" customFormat="1" ht="13.5" spans="1:9">
       <c r="A78" s="6"/>
       <c r="B78" s="20" t="s">
-        <v>257</v>
+        <v>299</v>
       </c>
       <c r="C78" s="21" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D78" s="13"/>
       <c r="E78" s="14" t="s">
@@ -49499,10 +51336,10 @@
     <row r="79" customFormat="1" ht="13.5" spans="1:9">
       <c r="A79" s="6"/>
       <c r="B79" s="20" t="s">
-        <v>258</v>
+        <v>300</v>
       </c>
       <c r="C79" s="21" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D79" s="13"/>
       <c r="E79" s="14" t="s">
@@ -49522,10 +51359,10 @@
     <row r="80" customFormat="1" ht="13.5" spans="1:9">
       <c r="A80" s="6"/>
       <c r="B80" s="20" t="s">
-        <v>259</v>
+        <v>301</v>
       </c>
       <c r="C80" s="21" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D80" s="13"/>
       <c r="E80" s="14" t="s">
@@ -49544,16 +51381,16 @@
     </row>
     <row r="81" customFormat="1" ht="13.5" customHeight="1" spans="1:9">
       <c r="A81" s="6" t="s">
-        <v>260</v>
+        <v>302</v>
       </c>
       <c r="B81" s="7" t="s">
         <v>158</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D81" s="13" t="s">
-        <v>261</v>
+        <v>303</v>
       </c>
       <c r="E81" s="14" t="s">
         <v>13</v>
@@ -49575,7 +51412,7 @@
         <v>160</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D82" s="13"/>
       <c r="E82" s="14" t="s">
@@ -49598,7 +51435,7 @@
         <v>161</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D83" s="13"/>
       <c r="E83" s="14" t="s">
@@ -49621,7 +51458,7 @@
         <v>162</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D84" s="13"/>
       <c r="E84" s="14" t="s">
@@ -49640,16 +51477,16 @@
     </row>
     <row r="85" customFormat="1" ht="13.5" customHeight="1" spans="1:9">
       <c r="A85" s="6" t="s">
-        <v>262</v>
+        <v>304</v>
       </c>
       <c r="B85" s="11" t="s">
-        <v>263</v>
+        <v>305</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D85" s="13" t="s">
-        <v>264</v>
+        <v>306</v>
       </c>
       <c r="E85" s="14" t="s">
         <v>13</v>
@@ -49668,10 +51505,10 @@
     <row r="86" customFormat="1" ht="13.5" spans="1:9">
       <c r="A86" s="6"/>
       <c r="B86" s="11" t="s">
-        <v>265</v>
+        <v>307</v>
       </c>
       <c r="C86" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D86" s="13"/>
       <c r="E86" s="14" t="s">
@@ -49691,10 +51528,10 @@
     <row r="87" customFormat="1" ht="13.5" spans="1:9">
       <c r="A87" s="6"/>
       <c r="B87" s="7" t="s">
-        <v>266</v>
+        <v>308</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D87" s="13"/>
       <c r="E87" s="14" t="s">
@@ -49714,10 +51551,10 @@
     <row r="88" customFormat="1" ht="13.5" spans="1:9">
       <c r="A88" s="6"/>
       <c r="B88" s="7" t="s">
-        <v>267</v>
+        <v>309</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D88" s="13"/>
       <c r="E88" s="14" t="s">
@@ -49737,10 +51574,10 @@
     <row r="89" customFormat="1" ht="13.5" spans="1:9">
       <c r="A89" s="6"/>
       <c r="B89" s="11" t="s">
-        <v>268</v>
+        <v>310</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D89" s="13"/>
       <c r="E89" s="14" t="s">
@@ -49760,10 +51597,10 @@
     <row r="90" spans="1:9">
       <c r="A90" s="6"/>
       <c r="B90" s="11" t="s">
-        <v>269</v>
+        <v>311</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D90" s="13"/>
       <c r="E90" s="14" t="s">
@@ -49783,10 +51620,10 @@
     <row r="91" spans="1:9">
       <c r="A91" s="6"/>
       <c r="B91" s="11" t="s">
-        <v>270</v>
+        <v>312</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D91" s="13"/>
       <c r="E91" s="14" t="s">
@@ -49806,10 +51643,10 @@
     <row r="92" spans="1:9">
       <c r="A92" s="6"/>
       <c r="B92" s="11" t="s">
-        <v>271</v>
+        <v>313</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D92" s="13"/>
       <c r="E92" s="14" t="s">
@@ -49829,10 +51666,10 @@
     <row r="93" spans="1:9">
       <c r="A93" s="6"/>
       <c r="B93" s="11" t="s">
-        <v>272</v>
+        <v>314</v>
       </c>
       <c r="C93" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D93" s="13"/>
       <c r="E93" s="14" t="s">
@@ -49851,16 +51688,16 @@
     </row>
     <row r="94" ht="13.5" customHeight="1" spans="1:9">
       <c r="A94" s="6" t="s">
-        <v>273</v>
+        <v>315</v>
       </c>
       <c r="B94" s="7" t="s">
         <v>158</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D94" s="13" t="s">
-        <v>274</v>
+        <v>316</v>
       </c>
       <c r="E94" s="14" t="s">
         <v>13</v>
@@ -49875,7 +51712,7 @@
         <v>13</v>
       </c>
       <c r="I94" s="18" t="s">
-        <v>275</v>
+        <v>317</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -49884,7 +51721,7 @@
         <v>160</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D95" s="13"/>
       <c r="E95" s="14" t="s">
@@ -49900,7 +51737,7 @@
         <v>13</v>
       </c>
       <c r="I95" s="18" t="s">
-        <v>275</v>
+        <v>317</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -49909,7 +51746,7 @@
         <v>161</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D96" s="13"/>
       <c r="E96" s="14" t="s">
@@ -49925,7 +51762,7 @@
         <v>13</v>
       </c>
       <c r="I96" s="18" t="s">
-        <v>275</v>
+        <v>317</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -49934,7 +51771,7 @@
         <v>162</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D97" s="13"/>
       <c r="E97" s="14" t="s">
@@ -49950,21 +51787,21 @@
         <v>13</v>
       </c>
       <c r="I97" s="18" t="s">
-        <v>275</v>
+        <v>317</v>
       </c>
     </row>
     <row r="98" ht="13.5" customHeight="1" spans="1:9">
       <c r="A98" s="22" t="s">
-        <v>276</v>
+        <v>318</v>
       </c>
       <c r="B98" s="7" t="s">
         <v>158</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D98" s="23" t="s">
-        <v>277</v>
+        <v>319</v>
       </c>
       <c r="E98" s="14" t="s">
         <v>13</v>
@@ -49986,7 +51823,7 @@
         <v>160</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D99" s="23"/>
       <c r="E99" s="14" t="s">
@@ -50009,7 +51846,7 @@
         <v>161</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D100" s="23"/>
       <c r="E100" s="14" t="s">
@@ -50032,7 +51869,7 @@
         <v>162</v>
       </c>
       <c r="C101" s="25" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D101" s="23"/>
       <c r="E101" s="26" t="s">

</xml_diff>